<commit_message>
kelas jalan, ruas kecamatan, drp
</commit_message>
<xml_diff>
--- a/database/seeders/data/LinkClass.xlsx
+++ b/database/seeders/data/LinkClass.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="LinkClass"/>
   </sheets>
   <definedNames>
-    <definedName name="LinkClass">'LinkClass'!$A$1:$E$5</definedName>
+    <definedName name="LinkClass">'LinkClass'!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -343,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -441,16 +441,16 @@
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>350900000277</t>
+          <t>350900000047</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" s="0">
-        <v>5.55000019073486</v>
+        <v>0.620000004768372</v>
       </c>
     </row>
     <row outlineLevel="0" r="5">
@@ -466,15 +466,215 @@
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
+          <t>350900000047</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E5" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>350900000157</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E6" s="0">
+        <v>0.800000011920929</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>350900000157</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E7" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>350900000157</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E8" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>350900000157</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E9" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>350900000160</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E10" s="0">
+        <v>1.77999997138977</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>350900000163</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E11" s="0">
+        <v>3.29999995231628</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>350900000277</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E12" s="0">
+        <v>5.55000019073486</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
           <t>350900000278</t>
         </is>
       </c>
-      <c r="D5" s="0" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E5" s="0">
+      <c r="E13" s="0">
         <v>2.96399998664856</v>
       </c>
     </row>

</xml_diff>